<commit_message>
modify map to make prd
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="5780" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,9 @@
     <t>address</t>
   </si>
   <si>
-    <t>西港雅苑</t>
-  </si>
-  <si>
     <t>xigangyayuan.jpg</t>
   </si>
   <si>
-    <t>恒大城</t>
-  </si>
-  <si>
     <t>hengdacheng.jpg</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>2009-12-10</t>
   </si>
   <si>
-    <t>紫薇希望城</t>
-  </si>
-  <si>
     <t>ziweixiwangcheng.jpg</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>城北凤城五路未央路与太华北路之间</t>
   </si>
   <si>
-    <t>曲江风景线</t>
-  </si>
-  <si>
     <t>qujiangfengjingxian.jpg</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
     <t>2012-10-01</t>
   </si>
   <si>
-    <t>兰蒂斯城</t>
-  </si>
-  <si>
     <t>landisicheng.jpg</t>
   </si>
   <si>
@@ -151,9 +136,6 @@
   </si>
   <si>
     <t>chanbabandao.jpg</t>
-  </si>
-  <si>
-    <t>浐灞半岛</t>
   </si>
   <si>
     <r>
@@ -196,9 +178,6 @@
     <t>‘2011-11-23</t>
   </si>
   <si>
-    <t>紫薇田园都市</t>
-  </si>
-  <si>
     <t>ziweitianyuandushi.jpg</t>
   </si>
   <si>
@@ -218,6 +197,27 @@
   </si>
   <si>
     <t>2002-07-28</t>
+  </si>
+  <si>
+    <t>铅锌冶炼企业一</t>
+  </si>
+  <si>
+    <t>铅锌冶炼企业二</t>
+  </si>
+  <si>
+    <t>铜冶炼企业一</t>
+  </si>
+  <si>
+    <t>金矿采选企业一</t>
+  </si>
+  <si>
+    <t>金矿采选企业二</t>
+  </si>
+  <si>
+    <t>钨钼冶炼企业一</t>
+  </si>
+  <si>
+    <t>钨钼冶炼企业二</t>
   </si>
 </sst>
 </file>
@@ -708,13 +708,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
@@ -740,246 +740,246 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5">
         <v>34.246433000000003</v>
       </c>
       <c r="C2" s="5">
-        <v>108.86695899999999</v>
+        <v>107.86695899999999</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
+      <c r="A3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="5">
         <v>34.192422999999998</v>
       </c>
       <c r="C3" s="5">
-        <v>108.870649</v>
+        <v>107.870649</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6">
         <v>34.343435999999997</v>
       </c>
       <c r="C4" s="6">
-        <v>108.951373</v>
+        <v>107.15137300000001</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="J4" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B5" s="17">
         <v>34.206408000000003</v>
       </c>
       <c r="C5" s="6">
-        <v>108.991241</v>
+        <v>107.19124100000001</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B6" s="20">
         <v>34.254626999999999</v>
       </c>
       <c r="C6" s="17">
-        <v>108.99767900000001</v>
+        <v>107.19767899999999</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B7" s="17">
         <v>34.312815999999998</v>
       </c>
       <c r="C7" s="6">
-        <v>109.04342699999999</v>
+        <v>107.04342699999999</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B8" s="17">
         <v>34.177227999999999</v>
       </c>
       <c r="C8" s="17">
-        <v>108.876572</v>
+        <v>107.876572</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>